<commit_message>
working on improving tailing file
</commit_message>
<xml_diff>
--- a/data/Yting_260321_20210326-103027/PrBlank.xlsx
+++ b/data/Yting_260321_20210326-103027/PrBlank.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Lab. #</t>
   </si>
@@ -43,22 +43,37 @@
     <t>Th-229</t>
   </si>
   <si>
-    <t>10815a</t>
+    <t>10815a_1</t>
   </si>
   <si>
     <t>11069b</t>
   </si>
   <si>
+    <t>10815a_2</t>
+  </si>
+  <si>
     <t>11070a</t>
   </si>
   <si>
+    <t>10815a_3</t>
+  </si>
+  <si>
     <t>11071a</t>
   </si>
   <si>
+    <t>10815a_4</t>
+  </si>
+  <si>
     <t>11072a</t>
   </si>
   <si>
+    <t>10815a_5</t>
+  </si>
+  <si>
     <t>11074b</t>
+  </si>
+  <si>
+    <t>10815a_6</t>
   </si>
 </sst>
 </file>
@@ -108,10 +123,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -414,7 +429,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
@@ -483,38 +498,38 @@
         <v>6.047727044813169</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>1.722393660559806E-06</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>7.416730505860654</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1.999779772135345E-05</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>3.545416565458131E-06</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>0.001667390641011717</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>5.985499732564791</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>3.789679319592728E-05</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>5.300997941212736</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>1.05708254967221E-05</v>
@@ -541,38 +556,38 @@
         <v>6.17218187404915</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="5" spans="1:9" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
         <v>1.269047629854621E-05</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>3.309720566616586</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1.748368770926484E-05</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
         <v>0.001390797904252803</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>2.48002163818169</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>1.68638325229282E-05</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>4.927633410776611</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>2.274696792101676E-06</v>
@@ -599,38 +614,38 @@
         <v>1.69180774144686</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
+    <row r="7" spans="1:9" s="1" customFormat="1">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
         <v>3.931994696179977</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1.027367194321486E-05</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>9.375688437993861E-07</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>0.00128441115512098</v>
       </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
         <v>2.562991537394842</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>1.022748519293807E-06</v>
@@ -657,38 +672,38 @@
         <v>5.674362497760528</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
+    <row r="9" spans="1:9" s="1" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
         <v>3.226750642478661</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>4.080199399118015E-06</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>1.368688666761227E-06</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>0.001284857472570258</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>1.878489970761384</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>1.189060425307813E-05</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>2.065172219659654</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -715,61 +730,61 @@
         <v>3.558630190272994</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
+    <row r="11" spans="1:9" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <v>3.724569987908039</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>1.132352587218959E-05</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>5.25031428721833E-06</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>0.00140329251599294</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>0.2981729973128998</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>3.715038300608196E-06</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>2.562991527899692</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
+    <row r="12" spans="1:9" s="2" customFormat="1">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
         <v>3.434175364993326</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>8.716663754905833E-06</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>3.46703067582153E-06</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>0.001248951895121897</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>2.148142098299981</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>1.523185468947675E-06</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="2">
         <v>2.065172207790717</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed tailing file median and std of intensities added
</commit_message>
<xml_diff>
--- a/data/Yting_260321_20210326-103027/PrBlank.xlsx
+++ b/data/Yting_260321_20210326-103027/PrBlank.xlsx
@@ -585,32 +585,32 @@
         <v>4.927633410776611</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:9" s="2" customFormat="1">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>2.274696792101676E-06</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>0.6961691431658217</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>2.740440369311263E-06</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>5.156479118359813E-06</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>0.001087274201883008</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>0.322804676821965</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>1.346776205468505E-06</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="2">
         <v>1.69180774144686</v>
       </c>
     </row>
@@ -759,32 +759,32 @@
         <v>2.562991527899692</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <v>3.434175364993326</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>8.716663754905833E-06</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>3.46703067582153E-06</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>0.001248951895121897</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>2.148142098299981</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>1.523185468947675E-06</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>2.065172207790717</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed redundant slope constant
</commit_message>
<xml_diff>
--- a/data/Yting_260321_20210326-103027/PrBlank.xlsx
+++ b/data/Yting_260321_20210326-103027/PrBlank.xlsx
@@ -585,32 +585,32 @@
         <v>4.927633410776611</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:9" s="1" customFormat="1">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>2.274696792101676E-06</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.6961691431658217</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>2.740440369311263E-06</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>5.156479118359813E-06</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>0.001087274201883008</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>0.322804676821965</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>1.346776205468505E-06</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>1.69180774144686</v>
       </c>
     </row>
@@ -643,32 +643,32 @@
         <v>2.562991537394842</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:9" s="2" customFormat="1">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>1.022748519293807E-06</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>2.065172229946067</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>1.244266159631219E-05</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>6.894880089227548E-06</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>0.001104335186357577</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>2.625218944396932</v>
       </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
         <v>5.674362497760528</v>
       </c>
     </row>

</xml_diff>